<commit_message>
Generated excel file from PDF content
</commit_message>
<xml_diff>
--- a/pdfs/20230301_Weekly_Epi_Update_132.xlsx
+++ b/pdfs/20230301_Weekly_Epi_Update_132.xlsx
@@ -5,99 +5,181 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="fields" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="country_cases_summarized_0" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="country_cases_summarized_1" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="country_cases_summarized_2" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="country_cases_summarized_3" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="country_cases_summarized_4" state="visible" r:id="rId9"/>
-    <sheet sheetId="7" name="country_cases_summarized" state="visible" r:id="rId10"/>
+    <sheet sheetId="2" name="newly_reported_covid_19_cases" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
-  <si>
-    <t>_source_country_cases</t>
-  </si>
-  <si>
-    <t>country_cases_summarized</t>
-  </si>
-  <si>
-    <t>At the country level, the highest numbers of new 28-day cases were reported from the United States of America (1 085 170 new cases; -29%), Japan (752 935 new cases; -77%), China (537 561 new cases; -95%), Germany (376 450 new cases; +6%), and the Republic of Korea (349 277 new cases; -66%). The highest numbers of new 28-day deaths were reported from the United States of America (12 111 new deaths; -17%), China (5915 new</t>
-  </si>
-  <si>
-    <t>SHEET: country_cases_summarized</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>number_of_newly_reported_cases</t>
-  </si>
-  <si>
-    <t>percentage_change_in_newly_reported_cases</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>1085170</t>
-  </si>
-  <si>
-    <t>-29</t>
-  </si>
-  <si>
-    <t>Japan</t>
-  </si>
-  <si>
-    <t>752935</t>
-  </si>
-  <si>
-    <t>-77</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>537561</t>
-  </si>
-  <si>
-    <t>-95</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>376450</t>
-  </si>
-  <si>
-    <t>+6</t>
-  </si>
-  <si>
-    <t>Republic of Korea</t>
-  </si>
-  <si>
-    <t>349277</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+  <si>
+    <t>newly_reported_covid_19_cases</t>
+  </si>
+  <si>
+    <t>SHEET: newly_reported_covid_19_cases</t>
+  </si>
+  <si>
+    <t>WHO_Region</t>
+  </si>
+  <si>
+    <t>new_cases_in_28_days</t>
+  </si>
+  <si>
+    <t>change_in_new_cases_in_28_days_(%)</t>
+  </si>
+  <si>
+    <t>cumulative_cases</t>
+  </si>
+  <si>
+    <t>new_deaths_in_28_days</t>
+  </si>
+  <si>
+    <t>change_in_new_deaths_in_28_days_(%)</t>
+  </si>
+  <si>
+    <t>cumulative_deaths</t>
+  </si>
+  <si>
+    <t>Western Pacific</t>
+  </si>
+  <si>
+    <t>1767793 (37%)</t>
+  </si>
+  <si>
+    <t>-89</t>
+  </si>
+  <si>
+    <t>201 174 961 (27%)</t>
+  </si>
+  <si>
+    <t>12132 (31%)</t>
+  </si>
+  <si>
+    <t>-84</t>
+  </si>
+  <si>
+    <t>405 082 (6%)</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t>549542 (32%)</t>
+  </si>
+  <si>
+    <t>-38</t>
+  </si>
+  <si>
+    <t>190 330 981 (25%)</t>
+  </si>
+  <si>
+    <t>17 208 (43%)</t>
+  </si>
+  <si>
+    <t>-22</t>
+  </si>
+  <si>
+    <t>2 931 207 (43%)</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>1 474 354 (31%)</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>273 198 084 (36%)</t>
+  </si>
+  <si>
+    <t>9784 (25%)</t>
+  </si>
+  <si>
+    <t>-44</t>
+  </si>
+  <si>
+    <t>2 193 431 (32%)</t>
+  </si>
+  <si>
+    <t>Eastern Mediterranean</t>
+  </si>
+  <si>
+    <t>15 103 (&lt;1%)</t>
+  </si>
+  <si>
+    <t>23 257 697 (3%)</t>
+  </si>
+  <si>
+    <t>238 (1%)</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>349 528 (5%)</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>14 258 (&lt;1%)</t>
+  </si>
+  <si>
+    <t>-53</t>
+  </si>
+  <si>
+    <t>9 497 673 (1%)</t>
+  </si>
+  <si>
+    <t>37 (&lt;1%)</t>
   </si>
   <si>
     <t>-66</t>
   </si>
   <si>
-    <t>SHEET: country_cases_summarized_0</t>
-  </si>
-  <si>
-    <t>SHEET: country_cases_summarized_1</t>
-  </si>
-  <si>
-    <t>SHEET: country_cases_summarized_2</t>
-  </si>
-  <si>
-    <t>SHEET: country_cases_summarized_3</t>
-  </si>
-  <si>
-    <t>SHEET: country_cases_summarized_4</t>
+    <t>175 295 (3%)</t>
+  </si>
+  <si>
+    <t>South-East Asia</t>
+  </si>
+  <si>
+    <t>10 971 (&lt;1%)</t>
+  </si>
+  <si>
+    <t>-36</t>
+  </si>
+  <si>
+    <t>60 766 335 (8%)</t>
+  </si>
+  <si>
+    <t>186 (&lt;1%)</t>
+  </si>
+  <si>
+    <t>-57</t>
+  </si>
+  <si>
+    <t>803 843 (12%)</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>832 021 (100%)</t>
+  </si>
+  <si>
+    <t>-76</t>
+  </si>
+  <si>
+    <t>758 226 495 (100%)</t>
+  </si>
+  <si>
+    <t>39 585 (100%)</t>
+  </si>
+  <si>
+    <t>6 858 399 (100%)</t>
   </si>
 </sst>
 </file>
@@ -474,23 +556,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -501,202 +577,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated gennerated excel file
</commit_message>
<xml_diff>
--- a/pdfs/20230301_Weekly_Epi_Update_132.xlsx
+++ b/pdfs/20230301_Weekly_Epi_Update_132.xlsx
@@ -20,166 +20,166 @@
     <t>SHEET: newly_reported_covid_19_cases</t>
   </si>
   <si>
-    <t>WHO_Region</t>
-  </si>
-  <si>
-    <t>new_cases_in_28_days</t>
-  </si>
-  <si>
-    <t>change_in_new_cases_in_28_days_(%)</t>
-  </si>
-  <si>
-    <t>cumulative_cases</t>
-  </si>
-  <si>
-    <t>new_deaths_in_28_days</t>
-  </si>
-  <si>
-    <t>change_in_new_deaths_in_28_days_(%)</t>
-  </si>
-  <si>
-    <t>cumulative_deaths</t>
+    <t>WHO Region</t>
+  </si>
+  <si>
+    <t>New cases in 28 days</t>
+  </si>
+  <si>
+    <t>Change in new cases in 28 days (%)</t>
+  </si>
+  <si>
+    <t>Cumulative cases</t>
+  </si>
+  <si>
+    <t>New deaths in 28 days</t>
+  </si>
+  <si>
+    <t>Change in new deaths in 28 days (%)</t>
+  </si>
+  <si>
+    <t>Cumulative deaths</t>
   </si>
   <si>
     <t>Western Pacific</t>
   </si>
   <si>
-    <t>1767793 (37%)</t>
-  </si>
-  <si>
-    <t>-89</t>
-  </si>
-  <si>
-    <t>201 174 961 (27%)</t>
-  </si>
-  <si>
-    <t>12132 (31%)</t>
-  </si>
-  <si>
-    <t>-84</t>
-  </si>
-  <si>
-    <t>405 082 (6%)</t>
+    <t xml:space="preserve">1767793 </t>
+  </si>
+  <si>
+    <t>-89%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201 174 961 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12132 </t>
+  </si>
+  <si>
+    <t>-84%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">405 082 </t>
   </si>
   <si>
     <t>Americas</t>
   </si>
   <si>
-    <t>549542 (32%)</t>
-  </si>
-  <si>
-    <t>-38</t>
-  </si>
-  <si>
-    <t>190 330 981 (25%)</t>
-  </si>
-  <si>
-    <t>17 208 (43%)</t>
-  </si>
-  <si>
-    <t>-22</t>
-  </si>
-  <si>
-    <t>2 931 207 (43%)</t>
+    <t xml:space="preserve">549542 </t>
+  </si>
+  <si>
+    <t>-38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">190 330 981 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 208 </t>
+  </si>
+  <si>
+    <t>-22%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 931 207 </t>
   </si>
   <si>
     <t>Europe</t>
   </si>
   <si>
-    <t>1 474 354 (31%)</t>
-  </si>
-  <si>
-    <t>-7</t>
-  </si>
-  <si>
-    <t>273 198 084 (36%)</t>
-  </si>
-  <si>
-    <t>9784 (25%)</t>
-  </si>
-  <si>
-    <t>-44</t>
-  </si>
-  <si>
-    <t>2 193 431 (32%)</t>
+    <t xml:space="preserve">1 474 354 </t>
+  </si>
+  <si>
+    <t>-7%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">273 198 084 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9784 </t>
+  </si>
+  <si>
+    <t>-44%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 193 431 </t>
   </si>
   <si>
     <t>Eastern Mediterranean</t>
   </si>
   <si>
-    <t>15 103 (&lt;1%)</t>
-  </si>
-  <si>
-    <t>23 257 697 (3%)</t>
-  </si>
-  <si>
-    <t>238 (1%)</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>349 528 (5%)</t>
+    <t xml:space="preserve">15 103 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 257 697 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">238 </t>
+  </si>
+  <si>
+    <t>18%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">349 528 </t>
   </si>
   <si>
     <t>Africa</t>
   </si>
   <si>
-    <t>14 258 (&lt;1%)</t>
-  </si>
-  <si>
-    <t>-53</t>
-  </si>
-  <si>
-    <t>9 497 673 (1%)</t>
-  </si>
-  <si>
-    <t>37 (&lt;1%)</t>
-  </si>
-  <si>
-    <t>-66</t>
-  </si>
-  <si>
-    <t>175 295 (3%)</t>
+    <t xml:space="preserve">14 258 </t>
+  </si>
+  <si>
+    <t>-53%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 497 673 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">37 </t>
+  </si>
+  <si>
+    <t>-66%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">175 295 </t>
   </si>
   <si>
     <t>South-East Asia</t>
   </si>
   <si>
-    <t>10 971 (&lt;1%)</t>
-  </si>
-  <si>
-    <t>-36</t>
-  </si>
-  <si>
-    <t>60 766 335 (8%)</t>
-  </si>
-  <si>
-    <t>186 (&lt;1%)</t>
-  </si>
-  <si>
-    <t>-57</t>
-  </si>
-  <si>
-    <t>803 843 (12%)</t>
+    <t xml:space="preserve">10 971 </t>
+  </si>
+  <si>
+    <t>-36%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 766 335 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">186 </t>
+  </si>
+  <si>
+    <t>-57%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">803 843 </t>
   </si>
   <si>
     <t>Global</t>
   </si>
   <si>
-    <t>832 021 (100%)</t>
-  </si>
-  <si>
-    <t>-76</t>
-  </si>
-  <si>
-    <t>758 226 495 (100%)</t>
-  </si>
-  <si>
-    <t>39 585 (100%)</t>
-  </si>
-  <si>
-    <t>6 858 399 (100%)</t>
+    <t xml:space="preserve">832 021 </t>
+  </si>
+  <si>
+    <t>-76%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">758 226 495 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 585 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 858 399 </t>
   </si>
 </sst>
 </file>

</xml_diff>